<commit_message>
calculations base set up
</commit_message>
<xml_diff>
--- a/files/SNE_IAC_Database.xlsx
+++ b/files/SNE_IAC_Database.xlsx
@@ -2579,7 +2579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD188"/>
+  <dimension ref="A1:AD189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14710,6 +14710,12 @@
         <is>
           <t>none</t>
         </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="K189">
+        <f>SUM(K2:K188)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -15729,7 +15735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15750,22 +15756,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Average_number_of_recommendations_per_assessment</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Total_recommended_savings</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Total_plant_energy_costs</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Total_number_of_recommendations_per_assessment</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Total_recommended_savings_per_assessment</t>
         </is>
       </c>
     </row>
@@ -15775,6 +15771,13 @@
       </c>
       <c r="B2" t="n">
         <v>187</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7.48</v>
+      </c>
+      <c r="D2">
+        <f>SUM(K2:K188)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>